<commit_message>
MOSIP-30683 Updated spanish languagle template for doc_type table
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_type.xlsx
+++ b/mosip_master/xlsx/doc_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015C37B5-C6D3-46E8-8B5E-67EFF4A8A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BF4D05-B22E-416D-BC71-0B78228F668B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="307">
   <si>
     <t>lang_code</t>
   </si>
@@ -918,9 +918,6 @@
     <t>Tarjeta PDS</t>
   </si>
   <si>
-    <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y ESIC</t>
-  </si>
-  <si>
     <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y también ESIC</t>
   </si>
   <si>
@@ -940,6 +937,18 @@
   </si>
   <si>
     <t>Tarjeta de Identidad de Referencia</t>
+  </si>
+  <si>
+    <t>Tarjeta de idintotificación de elector</t>
+  </si>
+  <si>
+    <t>Tarjeta de identificación de servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factura de </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarjeta médica emitida por el Gobierno del </t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4524,7 +4533,7 @@
         <v>61</v>
       </c>
       <c r="C188" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="D188" t="s">
         <v>282</v>
@@ -4541,7 +4550,7 @@
         <v>63</v>
       </c>
       <c r="C189" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D189" t="s">
         <v>283</v>
@@ -4694,7 +4703,7 @@
         <v>81</v>
       </c>
       <c r="C198" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="D198" t="s">
         <v>292</v>
@@ -4728,7 +4737,7 @@
         <v>85</v>
       </c>
       <c r="C200" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="D200" t="s">
         <v>294</v>
@@ -4762,10 +4771,10 @@
         <v>89</v>
       </c>
       <c r="C202" t="s">
+        <v>306</v>
+      </c>
+      <c r="D202" t="s">
         <v>296</v>
-      </c>
-      <c r="D202" t="s">
-        <v>297</v>
       </c>
       <c r="E202" t="b">
         <v>1</v>
@@ -4779,10 +4788,10 @@
         <v>92</v>
       </c>
       <c r="C203" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D203" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E203" t="b">
         <v>1</v>
@@ -4796,10 +4805,10 @@
         <v>94</v>
       </c>
       <c r="C204" t="s">
+        <v>298</v>
+      </c>
+      <c r="D204" t="s">
         <v>299</v>
-      </c>
-      <c r="D204" t="s">
-        <v>300</v>
       </c>
       <c r="E204" t="b">
         <v>1</v>
@@ -4816,7 +4825,7 @@
         <v>274</v>
       </c>
       <c r="D205" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E205" t="b">
         <v>1</v>
@@ -4830,10 +4839,10 @@
         <v>125</v>
       </c>
       <c r="C206" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D206" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E206" t="b">
         <v>1</v>
@@ -4847,10 +4856,10 @@
         <v>6</v>
       </c>
       <c r="C207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D207" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E207" t="b">
         <v>1</v>

</xml_diff>